<commit_message>
small changes to sample database
</commit_message>
<xml_diff>
--- a/data/faeces_sample_database.xlsx
+++ b/data/faeces_sample_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dida_\Dropbox\How to paper\HowToMetabarcoding\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387697DF-F073-4AC1-8315-37EAA2E630D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A057D5-D95A-413A-AC98-142C04D43C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1679" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="70">
   <si>
     <t>animal</t>
   </si>
@@ -251,12 +251,6 @@
   </si>
   <si>
     <t>ext mthd</t>
-  </si>
-  <si>
-    <t>343 </t>
-  </si>
-  <si>
-    <t>NEWSITE</t>
   </si>
 </sst>
 </file>
@@ -2157,7 +2151,7 @@
   <dimension ref="A1:FJ517"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" colorId="12" zoomScale="107" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B260" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
@@ -7307,7 +7301,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="129" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="129" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A129" s="12">
         <v>143</v>
       </c>
@@ -7341,7 +7335,7 @@
       <c r="CY129" s="6"/>
       <c r="CZ129" s="6"/>
     </row>
-    <row r="130" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="130" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A130" s="12">
         <v>144</v>
       </c>
@@ -7373,7 +7367,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="131" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="131" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A131" s="12">
         <v>145</v>
       </c>
@@ -7405,7 +7399,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="132" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="132" spans="1:104" s="5" customFormat="1" ht="16" customHeight="1">
       <c r="A132" s="12">
         <v>146</v>
       </c>
@@ -7418,16 +7412,16 @@
       <c r="D132" s="5">
         <v>2</v>
       </c>
-      <c r="E132" s="6">
+      <c r="E132" s="13">
         <v>2018</v>
       </c>
-      <c r="F132" s="6" t="s">
+      <c r="F132" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G132" s="2" t="s">
+      <c r="G132" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H132" s="2" t="s">
+      <c r="H132" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I132" s="7" t="s">
@@ -7436,164 +7430,10 @@
       <c r="J132" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="K132" s="31"/>
-      <c r="L132" s="31"/>
-      <c r="M132" s="31"/>
-      <c r="N132" s="31"/>
-      <c r="O132" s="31"/>
-      <c r="P132" s="31"/>
-      <c r="Q132" s="31"/>
-      <c r="R132" s="31"/>
-      <c r="S132" s="31"/>
-      <c r="T132" s="31"/>
-      <c r="U132" s="31"/>
-      <c r="V132" s="31"/>
-      <c r="W132" s="31"/>
-      <c r="X132" s="31"/>
-      <c r="Y132" s="31"/>
-      <c r="Z132" s="31"/>
-      <c r="AA132" s="31"/>
-      <c r="AB132" s="31"/>
-      <c r="AC132" s="31"/>
-      <c r="AD132" s="31"/>
-      <c r="AE132" s="31"/>
-      <c r="AF132" s="31"/>
-      <c r="AG132" s="31"/>
-      <c r="AH132" s="31"/>
-      <c r="AI132" s="31"/>
-      <c r="AJ132" s="31"/>
-      <c r="AK132" s="31"/>
-      <c r="AL132" s="31"/>
-      <c r="AM132" s="31"/>
-      <c r="AN132" s="31"/>
-      <c r="AO132" s="31"/>
-      <c r="AP132" s="31"/>
-      <c r="AQ132" s="31"/>
-      <c r="AR132" s="31"/>
-      <c r="AS132" s="31"/>
-      <c r="AT132" s="31"/>
-      <c r="AU132" s="31"/>
-      <c r="AV132" s="31"/>
-      <c r="AW132" s="31"/>
-      <c r="AX132" s="31"/>
-      <c r="AY132" s="31"/>
-      <c r="AZ132" s="31"/>
-      <c r="BA132" s="31"/>
-      <c r="BB132" s="31"/>
-      <c r="BC132" s="31"/>
-      <c r="BD132" s="31"/>
-      <c r="BE132" s="31"/>
-      <c r="BF132" s="31"/>
-      <c r="BG132" s="31"/>
-      <c r="BH132" s="31"/>
-      <c r="BI132" s="31"/>
-      <c r="BJ132" s="31"/>
-      <c r="BK132" s="31"/>
-      <c r="BL132" s="31"/>
-      <c r="BM132" s="31"/>
-      <c r="BN132" s="31"/>
-      <c r="BO132" s="31"/>
-      <c r="BP132" s="31"/>
-      <c r="BQ132" s="31"/>
-      <c r="BR132" s="31"/>
-      <c r="BS132" s="31"/>
-      <c r="BT132" s="31"/>
-      <c r="BU132" s="31"/>
-      <c r="BV132" s="31"/>
-      <c r="BW132" s="31"/>
-      <c r="BX132" s="31"/>
-      <c r="BY132" s="31"/>
-      <c r="BZ132" s="31"/>
-      <c r="CA132" s="31"/>
-      <c r="CB132" s="31"/>
-      <c r="CC132" s="31"/>
-      <c r="CD132" s="31"/>
-      <c r="CE132" s="31"/>
-      <c r="CF132" s="31"/>
-      <c r="CG132" s="31"/>
-      <c r="CH132" s="31"/>
-      <c r="CI132" s="31"/>
-      <c r="CJ132" s="31"/>
-      <c r="CK132" s="31"/>
-      <c r="CL132" s="31"/>
-      <c r="CM132" s="31"/>
-      <c r="CN132" s="31"/>
-      <c r="CO132" s="31"/>
-      <c r="CP132" s="31"/>
-      <c r="CQ132" s="31"/>
-      <c r="CR132" s="31"/>
-      <c r="CS132" s="31"/>
-      <c r="CT132" s="31"/>
-      <c r="CU132" s="31"/>
-      <c r="CV132" s="31"/>
-      <c r="CW132" s="31"/>
-      <c r="CX132" s="31"/>
-      <c r="CY132" s="32"/>
-      <c r="CZ132" s="32"/>
-      <c r="DA132" s="31"/>
-      <c r="DB132" s="31"/>
-      <c r="DC132" s="31"/>
-      <c r="DD132" s="31"/>
-      <c r="DE132" s="31"/>
-      <c r="DF132" s="31"/>
-      <c r="DG132" s="31"/>
-      <c r="DH132" s="31"/>
-      <c r="DI132" s="31"/>
-      <c r="DJ132" s="31"/>
-      <c r="DK132" s="31"/>
-      <c r="DL132" s="31"/>
-      <c r="DM132" s="31"/>
-      <c r="DN132" s="31"/>
-      <c r="DO132" s="31"/>
-      <c r="DP132" s="31"/>
-      <c r="DQ132" s="31"/>
-      <c r="DR132" s="31"/>
-      <c r="DS132" s="31"/>
-      <c r="DT132" s="31"/>
-      <c r="DU132" s="31"/>
-      <c r="DV132" s="31"/>
-      <c r="DW132" s="31"/>
-      <c r="DX132" s="31"/>
-      <c r="DY132" s="31"/>
-      <c r="DZ132" s="31"/>
-      <c r="EA132" s="31"/>
-      <c r="EB132" s="31"/>
-      <c r="EC132" s="31"/>
-      <c r="ED132" s="31"/>
-      <c r="EE132" s="31"/>
-      <c r="EF132" s="31"/>
-      <c r="EG132" s="31"/>
-      <c r="EH132" s="31"/>
-      <c r="EI132" s="31"/>
-      <c r="EJ132" s="31"/>
-      <c r="EK132" s="31"/>
-      <c r="EL132" s="31"/>
-      <c r="EM132" s="31"/>
-      <c r="EN132" s="31"/>
-      <c r="EO132" s="31"/>
-      <c r="EP132" s="31"/>
-      <c r="EQ132" s="31"/>
-      <c r="ER132" s="31"/>
-      <c r="ES132" s="31"/>
-      <c r="ET132" s="31"/>
-      <c r="EU132" s="31"/>
-      <c r="EV132" s="31"/>
-      <c r="EW132" s="31"/>
-      <c r="EX132" s="31"/>
-      <c r="EY132" s="31"/>
-      <c r="EZ132" s="31"/>
-      <c r="FA132" s="31"/>
-      <c r="FB132" s="31"/>
-      <c r="FC132" s="31"/>
-      <c r="FD132" s="31"/>
-      <c r="FE132" s="31"/>
-      <c r="FF132" s="31"/>
-      <c r="FG132" s="31"/>
-      <c r="FH132" s="31"/>
-      <c r="FI132" s="31"/>
-      <c r="FJ132" s="31"/>
-    </row>
-    <row r="133" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+      <c r="CY132" s="13"/>
+      <c r="CZ132" s="13"/>
+    </row>
+    <row r="133" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A133" s="12">
         <v>147</v>
       </c>
@@ -7625,7 +7465,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="134" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="134" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A134" s="12">
         <v>148</v>
       </c>
@@ -7659,7 +7499,7 @@
       <c r="CY134" s="6"/>
       <c r="CZ134" s="6"/>
     </row>
-    <row r="135" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="135" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A135" s="12">
         <v>149</v>
       </c>
@@ -7691,7 +7531,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="136" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="136" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A136" s="12">
         <v>150</v>
       </c>
@@ -7723,7 +7563,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="137" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="137" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A137" s="12">
         <v>151</v>
       </c>
@@ -7755,7 +7595,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="138" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="138" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A138" s="12">
         <v>152</v>
       </c>
@@ -7787,7 +7627,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="139" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="139" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A139" s="12">
         <v>153</v>
       </c>
@@ -7911,7 +7751,7 @@
       <c r="CW139" s="10"/>
       <c r="CX139" s="10"/>
     </row>
-    <row r="140" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="140" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A140" s="12">
         <v>154</v>
       </c>
@@ -7943,7 +7783,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="141" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="141" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A141" s="12">
         <v>155</v>
       </c>
@@ -7975,7 +7815,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="142" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="142" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A142" s="12">
         <v>158</v>
       </c>
@@ -8007,7 +7847,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="143" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="143" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A143" s="12">
         <v>159</v>
       </c>
@@ -8039,7 +7879,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="144" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="144" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A144" s="12">
         <v>163</v>
       </c>
@@ -15465,50 +15305,106 @@
     </row>
     <row r="255" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A255" s="12">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C255" s="5">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D255" s="5">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E255" s="6">
-        <v>2018</v>
-      </c>
-      <c r="F255" s="6" t="s">
-        <v>33</v>
+        <v>2017</v>
+      </c>
+      <c r="F255" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="G255" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H255" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I255" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J255" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="CY255" s="16"/>
-      <c r="CZ255" s="16"/>
+        <v>68</v>
+      </c>
+      <c r="DA255" s="10"/>
+      <c r="DB255" s="10"/>
+      <c r="DC255" s="10"/>
+      <c r="DD255" s="10"/>
+      <c r="DE255" s="10"/>
+      <c r="DF255" s="10"/>
+      <c r="DG255" s="10"/>
+      <c r="DH255" s="10"/>
+      <c r="DI255" s="10"/>
+      <c r="DJ255" s="10"/>
+      <c r="DK255" s="10"/>
+      <c r="DL255" s="10"/>
+      <c r="DM255" s="10"/>
+      <c r="DN255" s="10"/>
+      <c r="DO255" s="10"/>
+      <c r="DP255" s="10"/>
+      <c r="DQ255" s="10"/>
+      <c r="DR255" s="10"/>
+      <c r="DS255" s="10"/>
+      <c r="DT255" s="10"/>
+      <c r="DU255" s="10"/>
+      <c r="DV255" s="10"/>
+      <c r="DW255" s="10"/>
+      <c r="DX255" s="10"/>
+      <c r="DY255" s="10"/>
+      <c r="DZ255" s="10"/>
+      <c r="EA255" s="10"/>
+      <c r="EB255" s="10"/>
+      <c r="EC255" s="10"/>
+      <c r="ED255" s="10"/>
+      <c r="EE255" s="10"/>
+      <c r="EF255" s="10"/>
+      <c r="EG255" s="10"/>
+      <c r="EH255" s="10"/>
+      <c r="EI255" s="10"/>
+      <c r="EJ255" s="10"/>
+      <c r="EK255" s="10"/>
+      <c r="EL255" s="10"/>
+      <c r="EM255" s="10"/>
+      <c r="EN255" s="10"/>
+      <c r="EO255" s="10"/>
+      <c r="EP255" s="10"/>
+      <c r="EQ255" s="10"/>
+      <c r="ER255" s="10"/>
+      <c r="ES255" s="10"/>
+      <c r="ET255" s="10"/>
+      <c r="EU255" s="10"/>
+      <c r="EV255" s="10"/>
+      <c r="EW255" s="10"/>
+      <c r="EX255" s="10"/>
+      <c r="EY255" s="10"/>
+      <c r="EZ255" s="10"/>
+      <c r="FA255" s="10"/>
+      <c r="FB255" s="10"/>
+      <c r="FC255" s="10"/>
+      <c r="FD255" s="10"/>
+      <c r="FE255" s="10"/>
+      <c r="FF255" s="10"/>
     </row>
     <row r="256" spans="1:166" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A256" s="12">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C256" s="5">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D256" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E256" s="6">
         <v>2018</v>
@@ -15517,27 +15413,27 @@
         <v>33</v>
       </c>
       <c r="G256" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H256" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="I256" s="7" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="J256" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="257" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="257" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A257" s="12">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B257" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C257" s="5">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D257" s="5">
         <v>2</v>
@@ -15555,24 +15451,26 @@
         <v>11</v>
       </c>
       <c r="I257" s="7" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="J257" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="258" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+        <v>62</v>
+      </c>
+      <c r="CY257" s="16"/>
+      <c r="CZ257" s="16"/>
+    </row>
+    <row r="258" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A258" s="12">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B258" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C258" s="5">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D258" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E258" s="6">
         <v>2018</v>
@@ -15593,9 +15491,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="259" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="259" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A259" s="12">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B259" s="5" t="s">
         <v>1</v>
@@ -15625,9 +15523,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="260" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="260" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A260" s="12">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B260" s="5" t="s">
         <v>1</v>
@@ -15657,15 +15555,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="261" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="261" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A261" s="12">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B261" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C261" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D261" s="5">
         <v>2</v>
@@ -15689,24 +15587,24 @@
         <v>63</v>
       </c>
     </row>
-    <row r="262" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="262" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A262" s="12">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B262" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C262" s="5">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D262" s="5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E262" s="6">
-        <v>2017</v>
-      </c>
-      <c r="F262" s="13" t="s">
-        <v>32</v>
+        <v>2018</v>
+      </c>
+      <c r="F262" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="G262" s="2" t="s">
         <v>7</v>
@@ -15720,110 +15618,16 @@
       <c r="J262" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="K262" s="10"/>
-      <c r="L262" s="10"/>
-      <c r="M262" s="10"/>
-      <c r="N262" s="10"/>
-      <c r="O262" s="10"/>
-      <c r="P262" s="10"/>
-      <c r="Q262" s="10"/>
-      <c r="R262" s="10"/>
-      <c r="S262" s="10"/>
-      <c r="T262" s="10"/>
-      <c r="U262" s="10"/>
-      <c r="V262" s="10"/>
-      <c r="W262" s="10"/>
-      <c r="X262" s="10"/>
-      <c r="Y262" s="10"/>
-      <c r="Z262" s="10"/>
-      <c r="AA262" s="10"/>
-      <c r="AB262" s="10"/>
-      <c r="AC262" s="10"/>
-      <c r="AD262" s="10"/>
-      <c r="AE262" s="10"/>
-      <c r="AF262" s="10"/>
-      <c r="AG262" s="10"/>
-      <c r="AH262" s="10"/>
-      <c r="AI262" s="10"/>
-      <c r="AJ262" s="10"/>
-      <c r="AK262" s="10"/>
-      <c r="AL262" s="10"/>
-      <c r="AM262" s="10"/>
-      <c r="AN262" s="10"/>
-      <c r="AO262" s="10"/>
-      <c r="AP262" s="10"/>
-      <c r="AQ262" s="10"/>
-      <c r="AR262" s="10"/>
-      <c r="AS262" s="10"/>
-      <c r="AT262" s="10"/>
-      <c r="AU262" s="10"/>
-      <c r="AV262" s="10"/>
-      <c r="AW262" s="10"/>
-      <c r="AX262" s="10"/>
-      <c r="AY262" s="10"/>
-      <c r="AZ262" s="10"/>
-      <c r="BA262" s="10"/>
-      <c r="BB262" s="10"/>
-      <c r="BC262" s="10"/>
-      <c r="BD262" s="10"/>
-      <c r="BE262" s="10"/>
-      <c r="BF262" s="10"/>
-      <c r="BG262" s="10"/>
-      <c r="BH262" s="10"/>
-      <c r="BI262" s="10"/>
-      <c r="BJ262" s="10"/>
-      <c r="BK262" s="10"/>
-      <c r="BL262" s="10"/>
-      <c r="BM262" s="10"/>
-      <c r="BN262" s="10"/>
-      <c r="BO262" s="10"/>
-      <c r="BP262" s="10"/>
-      <c r="BQ262" s="10"/>
-      <c r="BR262" s="10"/>
-      <c r="BS262" s="10"/>
-      <c r="BT262" s="10"/>
-      <c r="BU262" s="10"/>
-      <c r="BV262" s="10"/>
-      <c r="BW262" s="10"/>
-      <c r="BX262" s="10"/>
-      <c r="BY262" s="10"/>
-      <c r="BZ262" s="10"/>
-      <c r="CA262" s="10"/>
-      <c r="CB262" s="10"/>
-      <c r="CC262" s="10"/>
-      <c r="CD262" s="10"/>
-      <c r="CE262" s="10"/>
-      <c r="CF262" s="10"/>
-      <c r="CG262" s="10"/>
-      <c r="CH262" s="10"/>
-      <c r="CI262" s="10"/>
-      <c r="CJ262" s="10"/>
-      <c r="CK262" s="10"/>
-      <c r="CL262" s="10"/>
-      <c r="CM262" s="10"/>
-      <c r="CN262" s="10"/>
-      <c r="CO262" s="10"/>
-      <c r="CP262" s="10"/>
-      <c r="CQ262" s="10"/>
-      <c r="CR262" s="10"/>
-      <c r="CS262" s="10"/>
-      <c r="CT262" s="10"/>
-      <c r="CU262" s="10"/>
-      <c r="CV262" s="10"/>
-      <c r="CW262" s="10"/>
-      <c r="CX262" s="6"/>
-      <c r="CY262" s="6"/>
-      <c r="CZ262" s="6"/>
-    </row>
-    <row r="263" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+    </row>
+    <row r="263" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A263" s="12">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B263" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C263" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D263" s="5">
         <v>2</v>
@@ -15847,24 +15651,24 @@
         <v>63</v>
       </c>
     </row>
-    <row r="264" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="264" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A264" s="12">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B264" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C264" s="5">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D264" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E264" s="6">
-        <v>2018</v>
-      </c>
-      <c r="F264" s="6" t="s">
-        <v>33</v>
+        <v>2017</v>
+      </c>
+      <c r="F264" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="G264" s="2" t="s">
         <v>7</v>
@@ -15873,15 +15677,109 @@
         <v>11</v>
       </c>
       <c r="I264" s="7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="J264" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="265" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+        <v>63</v>
+      </c>
+      <c r="K264" s="10"/>
+      <c r="L264" s="10"/>
+      <c r="M264" s="10"/>
+      <c r="N264" s="10"/>
+      <c r="O264" s="10"/>
+      <c r="P264" s="10"/>
+      <c r="Q264" s="10"/>
+      <c r="R264" s="10"/>
+      <c r="S264" s="10"/>
+      <c r="T264" s="10"/>
+      <c r="U264" s="10"/>
+      <c r="V264" s="10"/>
+      <c r="W264" s="10"/>
+      <c r="X264" s="10"/>
+      <c r="Y264" s="10"/>
+      <c r="Z264" s="10"/>
+      <c r="AA264" s="10"/>
+      <c r="AB264" s="10"/>
+      <c r="AC264" s="10"/>
+      <c r="AD264" s="10"/>
+      <c r="AE264" s="10"/>
+      <c r="AF264" s="10"/>
+      <c r="AG264" s="10"/>
+      <c r="AH264" s="10"/>
+      <c r="AI264" s="10"/>
+      <c r="AJ264" s="10"/>
+      <c r="AK264" s="10"/>
+      <c r="AL264" s="10"/>
+      <c r="AM264" s="10"/>
+      <c r="AN264" s="10"/>
+      <c r="AO264" s="10"/>
+      <c r="AP264" s="10"/>
+      <c r="AQ264" s="10"/>
+      <c r="AR264" s="10"/>
+      <c r="AS264" s="10"/>
+      <c r="AT264" s="10"/>
+      <c r="AU264" s="10"/>
+      <c r="AV264" s="10"/>
+      <c r="AW264" s="10"/>
+      <c r="AX264" s="10"/>
+      <c r="AY264" s="10"/>
+      <c r="AZ264" s="10"/>
+      <c r="BA264" s="10"/>
+      <c r="BB264" s="10"/>
+      <c r="BC264" s="10"/>
+      <c r="BD264" s="10"/>
+      <c r="BE264" s="10"/>
+      <c r="BF264" s="10"/>
+      <c r="BG264" s="10"/>
+      <c r="BH264" s="10"/>
+      <c r="BI264" s="10"/>
+      <c r="BJ264" s="10"/>
+      <c r="BK264" s="10"/>
+      <c r="BL264" s="10"/>
+      <c r="BM264" s="10"/>
+      <c r="BN264" s="10"/>
+      <c r="BO264" s="10"/>
+      <c r="BP264" s="10"/>
+      <c r="BQ264" s="10"/>
+      <c r="BR264" s="10"/>
+      <c r="BS264" s="10"/>
+      <c r="BT264" s="10"/>
+      <c r="BU264" s="10"/>
+      <c r="BV264" s="10"/>
+      <c r="BW264" s="10"/>
+      <c r="BX264" s="10"/>
+      <c r="BY264" s="10"/>
+      <c r="BZ264" s="10"/>
+      <c r="CA264" s="10"/>
+      <c r="CB264" s="10"/>
+      <c r="CC264" s="10"/>
+      <c r="CD264" s="10"/>
+      <c r="CE264" s="10"/>
+      <c r="CF264" s="10"/>
+      <c r="CG264" s="10"/>
+      <c r="CH264" s="10"/>
+      <c r="CI264" s="10"/>
+      <c r="CJ264" s="10"/>
+      <c r="CK264" s="10"/>
+      <c r="CL264" s="10"/>
+      <c r="CM264" s="10"/>
+      <c r="CN264" s="10"/>
+      <c r="CO264" s="10"/>
+      <c r="CP264" s="10"/>
+      <c r="CQ264" s="10"/>
+      <c r="CR264" s="10"/>
+      <c r="CS264" s="10"/>
+      <c r="CT264" s="10"/>
+      <c r="CU264" s="10"/>
+      <c r="CV264" s="10"/>
+      <c r="CW264" s="10"/>
+      <c r="CX264" s="6"/>
+      <c r="CY264" s="6"/>
+      <c r="CZ264" s="6"/>
+    </row>
+    <row r="265" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A265" s="12">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B265" s="5" t="s">
         <v>1</v>
@@ -15911,15 +15809,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="266" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="266" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A266" s="12">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B266" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C266" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D266" s="5">
         <v>2</v>
@@ -15937,18 +15835,18 @@
         <v>11</v>
       </c>
       <c r="I266" s="7" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="J266" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="267" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="267" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A267" s="12">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B267" s="5" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C267" s="5">
         <v>3</v>
@@ -15963,27 +15861,29 @@
         <v>33</v>
       </c>
       <c r="G267" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H267" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I267" s="7" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="J267" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="268" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+        <v>68</v>
+      </c>
+      <c r="CY267" s="6"/>
+      <c r="CZ267" s="6"/>
+    </row>
+    <row r="268" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A268" s="12">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B268" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C268" s="5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D268" s="5">
         <v>2</v>
@@ -16006,110 +15906,16 @@
       <c r="J268" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="K268" s="10"/>
-      <c r="L268" s="10"/>
-      <c r="M268" s="10"/>
-      <c r="N268" s="10"/>
-      <c r="O268" s="10"/>
-      <c r="P268" s="10"/>
-      <c r="Q268" s="10"/>
-      <c r="R268" s="10"/>
-      <c r="S268" s="10"/>
-      <c r="T268" s="10"/>
-      <c r="U268" s="10"/>
-      <c r="V268" s="10"/>
-      <c r="W268" s="10"/>
-      <c r="X268" s="10"/>
-      <c r="Y268" s="10"/>
-      <c r="Z268" s="10"/>
-      <c r="AA268" s="10"/>
-      <c r="AB268" s="10"/>
-      <c r="AC268" s="10"/>
-      <c r="AD268" s="10"/>
-      <c r="AE268" s="10"/>
-      <c r="AF268" s="10"/>
-      <c r="AG268" s="10"/>
-      <c r="AH268" s="10"/>
-      <c r="AI268" s="10"/>
-      <c r="AJ268" s="10"/>
-      <c r="AK268" s="10"/>
-      <c r="AL268" s="10"/>
-      <c r="AM268" s="10"/>
-      <c r="AN268" s="10"/>
-      <c r="AO268" s="10"/>
-      <c r="AP268" s="10"/>
-      <c r="AQ268" s="10"/>
-      <c r="AR268" s="10"/>
-      <c r="AS268" s="10"/>
-      <c r="AT268" s="10"/>
-      <c r="AU268" s="10"/>
-      <c r="AV268" s="10"/>
-      <c r="AW268" s="10"/>
-      <c r="AX268" s="10"/>
-      <c r="AY268" s="10"/>
-      <c r="AZ268" s="10"/>
-      <c r="BA268" s="10"/>
-      <c r="BB268" s="10"/>
-      <c r="BC268" s="10"/>
-      <c r="BD268" s="10"/>
-      <c r="BE268" s="10"/>
-      <c r="BF268" s="10"/>
-      <c r="BG268" s="10"/>
-      <c r="BH268" s="10"/>
-      <c r="BI268" s="10"/>
-      <c r="BJ268" s="10"/>
-      <c r="BK268" s="10"/>
-      <c r="BL268" s="10"/>
-      <c r="BM268" s="10"/>
-      <c r="BN268" s="10"/>
-      <c r="BO268" s="10"/>
-      <c r="BP268" s="10"/>
-      <c r="BQ268" s="10"/>
-      <c r="BR268" s="10"/>
-      <c r="BS268" s="10"/>
-      <c r="BT268" s="10"/>
-      <c r="BU268" s="10"/>
-      <c r="BV268" s="10"/>
-      <c r="BW268" s="10"/>
-      <c r="BX268" s="10"/>
-      <c r="BY268" s="10"/>
-      <c r="BZ268" s="10"/>
-      <c r="CA268" s="10"/>
-      <c r="CB268" s="10"/>
-      <c r="CC268" s="10"/>
-      <c r="CD268" s="10"/>
-      <c r="CE268" s="10"/>
-      <c r="CF268" s="10"/>
-      <c r="CG268" s="10"/>
-      <c r="CH268" s="10"/>
-      <c r="CI268" s="10"/>
-      <c r="CJ268" s="10"/>
-      <c r="CK268" s="10"/>
-      <c r="CL268" s="10"/>
-      <c r="CM268" s="10"/>
-      <c r="CN268" s="10"/>
-      <c r="CO268" s="10"/>
-      <c r="CP268" s="10"/>
-      <c r="CQ268" s="10"/>
-      <c r="CR268" s="10"/>
-      <c r="CS268" s="10"/>
-      <c r="CT268" s="10"/>
-      <c r="CU268" s="10"/>
-      <c r="CV268" s="10"/>
-      <c r="CW268" s="10"/>
-      <c r="CX268" s="6"/>
-      <c r="CY268" s="6"/>
-      <c r="CZ268" s="6"/>
-    </row>
-    <row r="269" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+    </row>
+    <row r="269" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A269" s="12">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B269" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C269" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D269" s="5">
         <v>2</v>
@@ -16127,15 +15933,15 @@
         <v>11</v>
       </c>
       <c r="I269" s="7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="J269" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="270" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="270" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A270" s="12">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="B270" s="5" t="s">
         <v>1</v>
@@ -16165,152 +15971,188 @@
         <v>63</v>
       </c>
     </row>
-    <row r="271" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+    <row r="271" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A271" s="12">
-        <v>324</v>
+        <v>341</v>
       </c>
       <c r="B271" s="5" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C271" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D271" s="5">
         <v>2</v>
       </c>
       <c r="E271" s="6">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="F271" s="6" t="s">
         <v>33</v>
       </c>
       <c r="G271" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H271" s="2" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="I271" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="J271" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="DA271" s="10"/>
-      <c r="DB271" s="10"/>
-      <c r="DC271" s="10"/>
-      <c r="DD271" s="10"/>
-      <c r="DE271" s="10"/>
-      <c r="DF271" s="10"/>
-      <c r="DG271" s="10"/>
-      <c r="DH271" s="10"/>
-      <c r="DI271" s="10"/>
-      <c r="DJ271" s="10"/>
-      <c r="DK271" s="10"/>
-      <c r="DL271" s="10"/>
-      <c r="DM271" s="10"/>
-      <c r="DN271" s="10"/>
-      <c r="DO271" s="10"/>
-      <c r="DP271" s="10"/>
-      <c r="DQ271" s="10"/>
-      <c r="DR271" s="10"/>
-      <c r="DS271" s="10"/>
-      <c r="DT271" s="10"/>
-      <c r="DU271" s="10"/>
-      <c r="DV271" s="10"/>
-      <c r="DW271" s="10"/>
-      <c r="DX271" s="10"/>
-      <c r="DY271" s="10"/>
-      <c r="DZ271" s="10"/>
-      <c r="EA271" s="10"/>
-      <c r="EB271" s="10"/>
-      <c r="EC271" s="10"/>
-      <c r="ED271" s="10"/>
-      <c r="EE271" s="10"/>
-      <c r="EF271" s="10"/>
-      <c r="EG271" s="10"/>
-      <c r="EH271" s="10"/>
-      <c r="EI271" s="10"/>
-      <c r="EJ271" s="10"/>
-      <c r="EK271" s="10"/>
-      <c r="EL271" s="10"/>
-      <c r="EM271" s="10"/>
-      <c r="EN271" s="10"/>
-      <c r="EO271" s="10"/>
-      <c r="EP271" s="10"/>
-      <c r="EQ271" s="10"/>
-      <c r="ER271" s="10"/>
-      <c r="ES271" s="10"/>
-      <c r="ET271" s="10"/>
-      <c r="EU271" s="10"/>
-      <c r="EV271" s="10"/>
-      <c r="EW271" s="10"/>
-      <c r="EX271" s="10"/>
-      <c r="EY271" s="10"/>
-      <c r="EZ271" s="10"/>
-      <c r="FA271" s="10"/>
-      <c r="FB271" s="10"/>
-      <c r="FC271" s="10"/>
-      <c r="FD271" s="10"/>
-      <c r="FE271" s="10"/>
-      <c r="FF271" s="10"/>
-    </row>
-    <row r="272" spans="1:162" s="9" customFormat="1" ht="16" customHeight="1">
+        <v>63</v>
+      </c>
+      <c r="K271" s="10"/>
+      <c r="L271" s="10"/>
+      <c r="M271" s="10"/>
+      <c r="N271" s="10"/>
+      <c r="O271" s="10"/>
+      <c r="P271" s="10"/>
+      <c r="Q271" s="10"/>
+      <c r="R271" s="10"/>
+      <c r="S271" s="10"/>
+      <c r="T271" s="10"/>
+      <c r="U271" s="10"/>
+      <c r="V271" s="10"/>
+      <c r="W271" s="10"/>
+      <c r="X271" s="10"/>
+      <c r="Y271" s="10"/>
+      <c r="Z271" s="10"/>
+      <c r="AA271" s="10"/>
+      <c r="AB271" s="10"/>
+      <c r="AC271" s="10"/>
+      <c r="AD271" s="10"/>
+      <c r="AE271" s="10"/>
+      <c r="AF271" s="10"/>
+      <c r="AG271" s="10"/>
+      <c r="AH271" s="10"/>
+      <c r="AI271" s="10"/>
+      <c r="AJ271" s="10"/>
+      <c r="AK271" s="10"/>
+      <c r="AL271" s="10"/>
+      <c r="AM271" s="10"/>
+      <c r="AN271" s="10"/>
+      <c r="AO271" s="10"/>
+      <c r="AP271" s="10"/>
+      <c r="AQ271" s="10"/>
+      <c r="AR271" s="10"/>
+      <c r="AS271" s="10"/>
+      <c r="AT271" s="10"/>
+      <c r="AU271" s="10"/>
+      <c r="AV271" s="10"/>
+      <c r="AW271" s="10"/>
+      <c r="AX271" s="10"/>
+      <c r="AY271" s="10"/>
+      <c r="AZ271" s="10"/>
+      <c r="BA271" s="10"/>
+      <c r="BB271" s="10"/>
+      <c r="BC271" s="10"/>
+      <c r="BD271" s="10"/>
+      <c r="BE271" s="10"/>
+      <c r="BF271" s="10"/>
+      <c r="BG271" s="10"/>
+      <c r="BH271" s="10"/>
+      <c r="BI271" s="10"/>
+      <c r="BJ271" s="10"/>
+      <c r="BK271" s="10"/>
+      <c r="BL271" s="10"/>
+      <c r="BM271" s="10"/>
+      <c r="BN271" s="10"/>
+      <c r="BO271" s="10"/>
+      <c r="BP271" s="10"/>
+      <c r="BQ271" s="10"/>
+      <c r="BR271" s="10"/>
+      <c r="BS271" s="10"/>
+      <c r="BT271" s="10"/>
+      <c r="BU271" s="10"/>
+      <c r="BV271" s="10"/>
+      <c r="BW271" s="10"/>
+      <c r="BX271" s="10"/>
+      <c r="BY271" s="10"/>
+      <c r="BZ271" s="10"/>
+      <c r="CA271" s="10"/>
+      <c r="CB271" s="10"/>
+      <c r="CC271" s="10"/>
+      <c r="CD271" s="10"/>
+      <c r="CE271" s="10"/>
+      <c r="CF271" s="10"/>
+      <c r="CG271" s="10"/>
+      <c r="CH271" s="10"/>
+      <c r="CI271" s="10"/>
+      <c r="CJ271" s="10"/>
+      <c r="CK271" s="10"/>
+      <c r="CL271" s="10"/>
+      <c r="CM271" s="10"/>
+      <c r="CN271" s="10"/>
+      <c r="CO271" s="10"/>
+      <c r="CP271" s="10"/>
+      <c r="CQ271" s="10"/>
+      <c r="CR271" s="10"/>
+      <c r="CS271" s="10"/>
+      <c r="CT271" s="10"/>
+      <c r="CU271" s="10"/>
+      <c r="CV271" s="10"/>
+      <c r="CW271" s="10"/>
+      <c r="CX271" s="6"/>
+      <c r="CY271" s="6"/>
+      <c r="CZ271" s="6"/>
+    </row>
+    <row r="272" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A272" s="12">
-        <v>325</v>
+        <v>342</v>
       </c>
       <c r="B272" s="5" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C272" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D272" s="5">
         <v>2</v>
       </c>
       <c r="E272" s="6">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="F272" s="6" t="s">
         <v>33</v>
       </c>
       <c r="G272" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H272" s="2" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="I272" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J272" s="7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="273" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A273" s="12">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="B273" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C273" s="5">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D273" s="5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E273" s="6">
         <v>2018</v>
       </c>
       <c r="F273" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G273" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H273" s="2" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="I273" s="7" t="s">
         <v>29</v>
@@ -16322,29 +16164,29 @@
       <c r="CZ273" s="6"/>
     </row>
     <row r="274" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
-      <c r="A274" s="12" t="s">
-        <v>70</v>
+      <c r="A274" s="12">
+        <v>345</v>
       </c>
       <c r="B274" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C274" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D274" s="5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E274" s="6">
         <v>2018</v>
       </c>
       <c r="F274" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G274" s="2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H274" s="2" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="I274" s="7" t="s">
         <v>29</v>
@@ -16352,39 +16194,37 @@
       <c r="J274" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="CY274" s="6"/>
-      <c r="CZ274" s="6"/>
     </row>
     <row r="275" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
       <c r="A275" s="12">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B275" s="5" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C275" s="5">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D275" s="5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E275" s="6">
         <v>2018</v>
       </c>
       <c r="F275" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G275" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H275" s="2" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="I275" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="J275" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="276" spans="1:104" s="9" customFormat="1" ht="16" customHeight="1">
@@ -21258,7 +21098,11 @@
       <c r="J517" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:FK519" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:FK519" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:FJ518">
+      <sortCondition ref="A1:A519"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:FJ518">
     <sortCondition ref="A2:A518"/>
   </sortState>

</xml_diff>